<commit_message>
add updating evidence file with tasks
</commit_message>
<xml_diff>
--- a/leonikaf/evidence.xlsx
+++ b/leonikaf/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb62f544338d7f5c/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{BE36E5FB-FBAE-4EAF-A37B-432A993CB3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{446F8F57-8DA1-46E0-A863-6AB4F4E8C909}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{BE36E5FB-FBAE-4EAF-A37B-432A993CB3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF26FAD6-2160-4942-A781-A46A80449FEA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -184,7 +184,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -198,6 +198,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -255,10 +262,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -645,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,25 +695,25 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H2" t="s">
@@ -715,7 +722,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -740,10 +747,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -774,10 +781,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -808,10 +815,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -842,10 +849,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -876,20 +883,20 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -920,20 +927,20 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -964,20 +971,20 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1008,20 +1015,20 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1052,20 +1059,20 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1096,20 +1103,20 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1141,10 +1148,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1175,20 +1182,20 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1219,20 +1226,20 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1259,12 +1266,12 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1291,12 +1298,12 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1323,12 +1330,12 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1355,12 +1362,12 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1396,13 +1403,13 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1442,16 +1449,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1491,16 +1498,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1540,16 +1547,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1590,16 +1597,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1632,10 +1639,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1649,8 +1656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,10 +1675,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>